<commit_message>
Made changes for filter
</commit_message>
<xml_diff>
--- a/sow_app/generated_excels/SOW-1437_Milestone_Payments.xlsx
+++ b/sow_app/generated_excels/SOW-1437_Milestone_Payments.xlsx
@@ -470,7 +470,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>SOW: SOW-1437 - client check</t>
+          <t>SOW: SOW-1437 - fo check</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Total Contract Value: $50,000.00</t>
+          <t>Total Contract Value: $10.00</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="7" t="n">
-        <v>15000</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="E11" s="8" t="n">
-        <v>15000</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">

</xml_diff>